<commit_message>
allowed many formerly generic hydro parameters to be specified for each individual plant; included initial filling level as user input
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6757E115-403B-4A53-98CA-016424DE890F}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A58FC77E-BCF1-4080-BA9C-9056D7F2C73E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
   <sheets>
     <sheet name="General parameters" sheetId="3" r:id="rId1"/>
@@ -18,18 +18,18 @@
     <sheet name="Simulation accuracy" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="alpha">'General parameters'!$B$6</definedName>
-    <definedName name="d_min">'General parameters'!$B$5</definedName>
-    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$10</definedName>
-    <definedName name="f_opt">'General parameters'!$B$9</definedName>
-    <definedName name="f_spill">'General parameters'!$B$10</definedName>
+    <definedName name="alpha">'Hydropower plant parameters'!$C$18</definedName>
+    <definedName name="d_min">'Hydropower plant parameters'!$C$17</definedName>
+    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$11</definedName>
+    <definedName name="f_opt">'Hydropower plant parameters'!$C$14</definedName>
+    <definedName name="f_spill">'Hydropower plant parameters'!$C$15</definedName>
     <definedName name="g">'General parameters'!$B$4</definedName>
-    <definedName name="gamma_hydro">'General parameters'!$B$7</definedName>
-    <definedName name="LOEE_allowed">'General parameters'!$B$12</definedName>
-    <definedName name="mu">'General parameters'!$B$8</definedName>
-    <definedName name="option_storage">'General parameters'!$B$13</definedName>
+    <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$19</definedName>
+    <definedName name="LOEE_allowed">'General parameters'!$B$6</definedName>
+    <definedName name="mu">'Hydropower plant parameters'!$C$20</definedName>
+    <definedName name="option_storage">'General parameters'!$B$7</definedName>
     <definedName name="rho">'General parameters'!$B$3</definedName>
-    <definedName name="T_fill_thres">'General parameters'!$B$11</definedName>
+    <definedName name="T_fill_thres">'General parameters'!$B$5</definedName>
     <definedName name="year_end">'General parameters'!$B$2</definedName>
     <definedName name="year_start">'General parameters'!$B$1</definedName>
   </definedNames>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>year_start</t>
   </si>
@@ -152,9 +152,6 @@
     <t>option_storage</t>
   </si>
   <si>
-    <t>minimum required environmental outflow fraction (eq. S4, S5)</t>
-  </si>
-  <si>
     <t>density of water (kg/m^3) (introduced in eq. S3)</t>
   </si>
   <si>
@@ -176,12 +173,6 @@
     <t>optimal filling fraction f_opt (eq. S4, S5)</t>
   </si>
   <si>
-    <t>threshold for determining whether HPP is "large" or "small"</t>
-  </si>
-  <si>
-    <t>wish to model pumped storage (Note 7) or not? (0 = no, 1 = yes)</t>
-  </si>
-  <si>
     <t>N_ELCC</t>
   </si>
   <si>
@@ -324,6 +315,27 @@
   </si>
   <si>
     <t>allowed Loss of Energy Expectation as percentage of yearly ELCC</t>
+  </si>
+  <si>
+    <t>V_initial_frac</t>
+  </si>
+  <si>
+    <t>initial filling fraction of lake volume</t>
+  </si>
+  <si>
+    <t>[if using pumped storage assessment] initial filling fraction of lower lake volume</t>
+  </si>
+  <si>
+    <t>V_lower_initial_frac</t>
+  </si>
+  <si>
+    <t>minimum required environmental outflow fraction of average inflow (eq. S4, S5)</t>
+  </si>
+  <si>
+    <t>represents number of years of filling as threshold for determining f_reg if left unspecified by user (see sheet "Hydropower plant parameters"). Default/recommended is unity, so f_reg represents the fraction of annual mean inflow that would take exactly one year to fill reservoir.</t>
+  </si>
+  <si>
+    <t>wish to activate pumped storage module (Note 7) for at least one hydropower plant or not? (0 = no, 1 = yes)</t>
   </si>
 </sst>
 </file>
@@ -373,11 +385,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
@@ -693,16 +708,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80D586F-189B-4452-92A0-B50C92D09EB9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -735,7 +750,7 @@
         <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -746,107 +761,40 @@
         <v>9.81</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0.1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>0.8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.95</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
+      <c r="C7" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -856,16 +804,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="2" max="2" width="47.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -873,7 +821,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>20</v>
@@ -884,10 +832,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -901,7 +849,7 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -915,7 +863,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>80</v>
@@ -929,7 +877,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1">
         <v>440000000</v>
@@ -943,7 +891,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1">
         <v>12570000000</v>
@@ -954,190 +902,304 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C7">
-        <v>400</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
-        <v>165</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="2">
-        <f>C7/(C9*rho*g*C4)*10^6</f>
-        <v>637.1049949031601</v>
-      </c>
-      <c r="D8" s="2">
-        <f>D7/(D9*rho*g*D4)*10^6</f>
-        <v>582.39514769540949</v>
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9">
-        <v>0.8</v>
-      </c>
-      <c r="D9">
-        <v>0.8</v>
+        <v>74</v>
+      </c>
+      <c r="C9" s="2">
+        <f>C8/(C10*rho*g*C4)*10^6</f>
+        <v>637.1049949031601</v>
+      </c>
+      <c r="D9" s="2">
+        <f>D8/(D10*rho*g*D4)*10^6</f>
+        <v>582.39514769540949</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11">
-        <v>0.1</v>
-      </c>
-      <c r="D11">
-        <v>0.1</v>
-      </c>
-    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C12">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D12">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13">
-        <v>90</v>
+        <v>0.2</v>
       </c>
       <c r="D13">
-        <v>90</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D14">
-        <v>0.74765197999999999</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>0.95</v>
+      </c>
+      <c r="D15">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.74765197999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D18">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>0.1</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="3">
         <f>C6/1000</f>
         <v>12570000</v>
       </c>
-      <c r="D15" t="e">
+      <c r="D22" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23">
+        <v>0.8</v>
+      </c>
+      <c r="D23" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
         <v>100</v>
       </c>
-      <c r="D16" t="e">
+      <c r="D24" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="2">
-        <f>C16/(C18^(-1)*rho*g*C4)*10^6</f>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2">
+        <f>C24/(C26^(-1)*rho*g*C4)*10^6</f>
         <v>101.9367991845056</v>
       </c>
-      <c r="D17" t="e">
+      <c r="D25" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18">
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26">
         <v>0.8</v>
       </c>
-      <c r="D18">
+      <c r="D26">
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19">
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D19">
+      <c r="D27">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
@@ -1163,134 +1225,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1">
         <v>1000</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0.2</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>0.2</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow the user to run tests on a flexible part of the entered time series to speed up simulation time
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A58FC77E-BCF1-4080-BA9C-9056D7F2C73E}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A06DD1FA-0A9D-4A50-BFC7-1C23AA0B612D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -23,13 +23,13 @@
     <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$11</definedName>
     <definedName name="f_opt">'Hydropower plant parameters'!$C$14</definedName>
     <definedName name="f_spill">'Hydropower plant parameters'!$C$15</definedName>
-    <definedName name="g">'General parameters'!$B$4</definedName>
+    <definedName name="g">'General parameters'!$B$5</definedName>
     <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$19</definedName>
-    <definedName name="LOEE_allowed">'General parameters'!$B$6</definedName>
+    <definedName name="LOEE_allowed">'General parameters'!$B$7</definedName>
     <definedName name="mu">'Hydropower plant parameters'!$C$20</definedName>
-    <definedName name="option_storage">'General parameters'!$B$7</definedName>
-    <definedName name="rho">'General parameters'!$B$3</definedName>
-    <definedName name="T_fill_thres">'General parameters'!$B$5</definedName>
+    <definedName name="option_storage">'General parameters'!$B$8</definedName>
+    <definedName name="rho">'General parameters'!$B$4</definedName>
+    <definedName name="T_fill_thres">'General parameters'!$B$6</definedName>
     <definedName name="year_end">'General parameters'!$B$2</definedName>
     <definedName name="year_start">'General parameters'!$B$1</definedName>
   </definedNames>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>year_start</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>wish to activate pumped storage module (Note 7) for at least one hydropower plant or not? (0 = no, 1 = yes)</t>
+  </si>
+  <si>
+    <t>column_start</t>
+  </si>
+  <si>
+    <t>index of column (first column = 1) corresponding to year_start in time series Excel sheets (this needs to be the same across all Excel sheets)</t>
   </si>
 </sst>
 </file>
@@ -708,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80D586F-189B-4452-92A0-B50C92D09EB9}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,58 +748,69 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="B3">
-        <v>1000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>9.81</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>17</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>31</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -806,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
allow easier modelling of various scenarios for the same hydropower plant in one simulation batch through dynamic sheet naming in "data_xxx" files
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A06DD1FA-0A9D-4A50-BFC7-1C23AA0B612D}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5EA085B-5EE8-473F-B64A-6891E03841D3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -18,15 +18,15 @@
     <sheet name="Simulation accuracy" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="alpha">'Hydropower plant parameters'!$C$18</definedName>
-    <definedName name="d_min">'Hydropower plant parameters'!$C$17</definedName>
-    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$11</definedName>
-    <definedName name="f_opt">'Hydropower plant parameters'!$C$14</definedName>
-    <definedName name="f_spill">'Hydropower plant parameters'!$C$15</definedName>
+    <definedName name="alpha">'Hydropower plant parameters'!$C$24</definedName>
+    <definedName name="d_min">'Hydropower plant parameters'!$C$23</definedName>
+    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$17</definedName>
+    <definedName name="f_opt">'Hydropower plant parameters'!$C$20</definedName>
+    <definedName name="f_spill">'Hydropower plant parameters'!$C$21</definedName>
     <definedName name="g">'General parameters'!$B$5</definedName>
-    <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$19</definedName>
+    <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$25</definedName>
     <definedName name="LOEE_allowed">'General parameters'!$B$7</definedName>
-    <definedName name="mu">'Hydropower plant parameters'!$C$20</definedName>
+    <definedName name="mu">'Hydropower plant parameters'!$C$26</definedName>
     <definedName name="option_storage">'General parameters'!$B$8</definedName>
     <definedName name="rho">'General parameters'!$B$4</definedName>
     <definedName name="T_fill_thres">'General parameters'!$B$6</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
   <si>
     <t>year_start</t>
   </si>
@@ -254,9 +254,6 @@
     <t>fraction</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>maximum head in m</t>
   </si>
   <si>
@@ -302,18 +299,12 @@
     <t>fraction of lake volume at which production restarts after stopping</t>
   </si>
   <si>
-    <t>HPP_name_timeseries</t>
-  </si>
-  <si>
     <t>f_reg</t>
   </si>
   <si>
     <t>[leave empty if unsure - default will be used] which fraction of the water is allocatable for regulated use</t>
   </si>
   <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull time series</t>
-  </si>
-  <si>
     <t>allowed Loss of Energy Expectation as percentage of yearly ELCC</t>
   </si>
   <si>
@@ -342,6 +333,33 @@
   </si>
   <si>
     <t>index of column (first column = 1) corresponding to year_start in time series Excel sheets (this needs to be the same across all Excel sheets)</t>
+  </si>
+  <si>
+    <t>HPP_name_data_CF_solar</t>
+  </si>
+  <si>
+    <t>HPP_name_data_CF_wind</t>
+  </si>
+  <si>
+    <t>HPP_name_data_evaporation</t>
+  </si>
+  <si>
+    <t>HPP_name_data_inflow</t>
+  </si>
+  <si>
+    <t>HPP_name_data_load</t>
+  </si>
+  <si>
+    <t>HPP_name_data_precipitation</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data</t>
+  </si>
+  <si>
+    <t>name of hydropower plant in simulation</t>
+  </si>
+  <si>
+    <t>HPP_name_data_bathymetry</t>
   </si>
 </sst>
 </file>
@@ -717,7 +735,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -750,13 +768,13 @@
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -789,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -800,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -811,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -821,15 +839,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.90625" customWidth="1"/>
     <col min="2" max="2" width="47.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -838,7 +856,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
         <v>20</v>
@@ -849,10 +867,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -863,360 +881,444 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4">
-        <v>80</v>
-      </c>
-      <c r="D4">
-        <v>36.1</v>
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="1">
-        <v>440000000</v>
-      </c>
-      <c r="D5" s="1">
-        <v>900000000</v>
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="1">
-        <v>12570000000</v>
-      </c>
-      <c r="D6" s="1">
-        <v>8300000000</v>
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7">
-        <v>0.8</v>
-      </c>
-      <c r="D7">
-        <v>0.8</v>
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>400</v>
-      </c>
-      <c r="D8">
-        <v>165</v>
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="2">
-        <f>C8/(C10*rho*g*C4)*10^6</f>
-        <v>637.1049949031601</v>
-      </c>
-      <c r="D9" s="2">
-        <f>D8/(D10*rho*g*D4)*10^6</f>
-        <v>582.39514769540949</v>
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C10">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="D10">
-        <v>0.8</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1">
+        <v>440000000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>900000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12570000000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8300000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13">
+        <v>0.8</v>
+      </c>
+      <c r="D13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+      <c r="D14">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2">
+        <f>C14/(C16*rho*g*C10)*10^6</f>
+        <v>637.1049949031601</v>
+      </c>
+      <c r="D15" s="2">
+        <f>D14/(D16*rho*g*D10)*10^6</f>
+        <v>582.39514769540949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16">
+        <v>0.8</v>
+      </c>
+      <c r="D16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11">
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D11">
+      <c r="D17">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12">
-        <v>0.1</v>
-      </c>
-      <c r="D12">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13">
-        <v>0.2</v>
-      </c>
-      <c r="D13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14">
-        <v>0.8</v>
-      </c>
-      <c r="D14">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15">
-        <v>0.95</v>
-      </c>
-      <c r="D15">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0.74765197999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17">
-        <v>0.1</v>
-      </c>
-      <c r="D17">
-        <v>0.1</v>
-      </c>
-    </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18">
+        <v>0.1</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>0.8</v>
+      </c>
+      <c r="D20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>0.95</v>
+      </c>
+      <c r="D21">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.74765197999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23">
+        <v>0.1</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B24" t="s">
         <v>34</v>
       </c>
-      <c r="C18">
+      <c r="C24">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D18">
+      <c r="D24">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20">
-        <v>0.1</v>
-      </c>
-      <c r="D20">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21">
-        <v>90</v>
-      </c>
-      <c r="D21">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3">
-        <f>C6/1000</f>
-        <v>12570000</v>
-      </c>
-      <c r="D22" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23">
-        <v>0.8</v>
-      </c>
-      <c r="D23" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-      <c r="D24" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="2">
-        <f>C24/(C26^(-1)*rho*g*C4)*10^6</f>
-        <v>101.9367991845056</v>
-      </c>
-      <c r="D25" t="e">
-        <v>#N/A</v>
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C26">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="D26">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>78</v>
       </c>
       <c r="C27">
+        <v>90</v>
+      </c>
+      <c r="D27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="3">
+        <f>C12/1000</f>
+        <v>12570000</v>
+      </c>
+      <c r="D28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29">
+        <v>0.8</v>
+      </c>
+      <c r="D29" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="2">
+        <f>C30/(C32^(-1)*rho*g*C10)*10^6</f>
+        <v>101.9367991845056</v>
+      </c>
+      <c r="D31" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32">
+        <v>0.8</v>
+      </c>
+      <c r="D32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D27">
+      <c r="D33">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
allow user to activate/disactivate hydropower plants in the list from Excel
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5EA085B-5EE8-473F-B64A-6891E03841D3}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49708EB3-948B-40EB-A4CF-3C9927BC7B74}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
   <sheets>
     <sheet name="General parameters" sheetId="3" r:id="rId1"/>
@@ -18,15 +18,15 @@
     <sheet name="Simulation accuracy" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="alpha">'Hydropower plant parameters'!$C$24</definedName>
-    <definedName name="d_min">'Hydropower plant parameters'!$C$23</definedName>
-    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$17</definedName>
-    <definedName name="f_opt">'Hydropower plant parameters'!$C$20</definedName>
-    <definedName name="f_spill">'Hydropower plant parameters'!$C$21</definedName>
+    <definedName name="alpha">'Hydropower plant parameters'!$C$25</definedName>
+    <definedName name="d_min">'Hydropower plant parameters'!$C$24</definedName>
+    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$18</definedName>
+    <definedName name="f_opt">'Hydropower plant parameters'!$C$21</definedName>
+    <definedName name="f_spill">'Hydropower plant parameters'!$C$22</definedName>
     <definedName name="g">'General parameters'!$B$5</definedName>
-    <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$25</definedName>
+    <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$26</definedName>
     <definedName name="LOEE_allowed">'General parameters'!$B$7</definedName>
-    <definedName name="mu">'Hydropower plant parameters'!$C$26</definedName>
+    <definedName name="mu">'Hydropower plant parameters'!$C$27</definedName>
     <definedName name="option_storage">'General parameters'!$B$8</definedName>
     <definedName name="rho">'General parameters'!$B$4</definedName>
     <definedName name="T_fill_thres">'General parameters'!$B$6</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>year_start</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>HPP_name_data_bathymetry</t>
+  </si>
+  <si>
+    <t>HPP_active</t>
+  </si>
+  <si>
+    <t>used to include (= 1) or exclude (= 0) plant from current run</t>
   </si>
 </sst>
 </file>
@@ -734,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80D586F-189B-4452-92A0-B50C92D09EB9}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -839,10 +845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -867,21 +873,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
+        <v>103</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>99</v>
@@ -895,7 +901,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -909,7 +915,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>99</v>
@@ -923,7 +929,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>99</v>
@@ -937,7 +943,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>99</v>
@@ -951,7 +957,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -965,300 +971,300 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>36.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="1">
-        <v>440000000</v>
-      </c>
-      <c r="D11" s="1">
-        <v>900000000</v>
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>36.1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1">
-        <v>12570000000</v>
+        <v>440000000</v>
       </c>
       <c r="D12" s="1">
-        <v>8300000000</v>
+        <v>900000000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13">
-        <v>0.8</v>
-      </c>
-      <c r="D13">
-        <v>0.8</v>
+        <v>68</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12570000000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8300000000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C14">
-        <v>400</v>
+        <v>0.8</v>
       </c>
       <c r="D14">
-        <v>165</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="2">
-        <f>C14/(C16*rho*g*C10)*10^6</f>
-        <v>637.1049949031601</v>
-      </c>
-      <c r="D15" s="2">
-        <f>D14/(D16*rho*g*D10)*10^6</f>
-        <v>582.39514769540949</v>
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>400</v>
+      </c>
+      <c r="D15">
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16">
-        <v>0.8</v>
-      </c>
-      <c r="D16">
-        <v>0.8</v>
+        <v>73</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C15/(C17*rho*g*C11)*10^6</f>
+        <v>637.1049949031601</v>
+      </c>
+      <c r="D16" s="2">
+        <f>D15/(D17*rho*g*D11)*10^6</f>
+        <v>582.39514769540949</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>0.8</v>
+      </c>
+      <c r="D17">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>75</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18">
-        <v>0.1</v>
-      </c>
-      <c r="D18">
-        <v>0.1</v>
-      </c>
-    </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D19">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C20">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D20">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="D21">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="D22">
-        <v>0.74765197999999999</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C23">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.1</v>
+        <v>0.74765197999999999</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
+        <v>0.1</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-      <c r="D25">
-        <v>10</v>
-      </c>
-    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="C27">
-        <v>90</v>
+        <v>0.1</v>
       </c>
       <c r="D27">
-        <v>90</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="3">
-        <f>C12/1000</f>
-        <v>12570000</v>
-      </c>
-      <c r="D28" t="e">
-        <v>#N/A</v>
+        <v>78</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29">
-        <v>0.8</v>
+        <v>70</v>
+      </c>
+      <c r="C29" s="3">
+        <f>C13/1000</f>
+        <v>12570000</v>
       </c>
       <c r="D29" t="e">
         <v>#N/A</v>
@@ -1266,13 +1272,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C30">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="D30" t="e">
         <v>#N/A</v>
@@ -1280,14 +1286,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="2">
-        <f>C30/(C32^(-1)*rho*g*C10)*10^6</f>
-        <v>101.9367991845056</v>
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
       </c>
       <c r="D31" t="e">
         <v>#N/A</v>
@@ -1295,30 +1300,45 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32">
-        <v>0.8</v>
-      </c>
-      <c r="D32">
-        <v>0.8</v>
+        <v>72</v>
+      </c>
+      <c r="C32" s="2">
+        <f>C31/(C33^(-1)*rho*g*C11)*10^6</f>
+        <v>101.9367991845056</v>
+      </c>
+      <c r="D32" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33">
+        <v>0.8</v>
+      </c>
+      <c r="D33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>15</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>77</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
removed spurious defined names from Excel file
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49708EB3-948B-40EB-A4CF-3C9927BC7B74}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB07566-2A5B-48AC-90DF-1B4D6B1DBCA4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -18,15 +18,8 @@
     <sheet name="Simulation accuracy" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="alpha">'Hydropower plant parameters'!$C$25</definedName>
-    <definedName name="d_min">'Hydropower plant parameters'!$C$24</definedName>
-    <definedName name="dP_ramp_turb">'Hydropower plant parameters'!$C$18</definedName>
-    <definedName name="f_opt">'Hydropower plant parameters'!$C$21</definedName>
-    <definedName name="f_spill">'Hydropower plant parameters'!$C$22</definedName>
     <definedName name="g">'General parameters'!$B$5</definedName>
-    <definedName name="gamma_hydro">'Hydropower plant parameters'!$C$26</definedName>
     <definedName name="LOEE_allowed">'General parameters'!$B$7</definedName>
-    <definedName name="mu">'Hydropower plant parameters'!$C$27</definedName>
     <definedName name="option_storage">'General parameters'!$B$8</definedName>
     <definedName name="rho">'General parameters'!$B$4</definedName>
     <definedName name="T_fill_thres">'General parameters'!$B$6</definedName>
@@ -848,7 +841,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
clarification of parameter c_solar_relative in simulation settings sheet
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB07566-2A5B-48AC-90DF-1B4D6B1DBCA4}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6E3016-6ECC-4688-9A7A-405F5D89763B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -244,9 +244,6 @@
     <t>Q_max_pump</t>
   </si>
   <si>
-    <t>fraction</t>
-  </si>
-  <si>
     <t>maximum head in m</t>
   </si>
   <si>
@@ -359,6 +356,9 @@
   </si>
   <si>
     <t>used to include (= 1) or exclude (= 0) plant from current run</t>
+  </si>
+  <si>
+    <t>fraction of solar in the solar/wind portfolio</t>
   </si>
 </sst>
 </file>
@@ -767,13 +767,13 @@
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +841,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,7 +855,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>20</v>
@@ -866,10 +866,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
         <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -880,10 +880,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -894,10 +894,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -908,10 +908,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -936,10 +936,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
         <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -950,10 +950,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -964,10 +964,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -981,7 +981,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -995,7 +995,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11">
         <v>80</v>
@@ -1009,7 +1009,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1">
         <v>440000000</v>
@@ -1023,7 +1023,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1">
         <v>12570000000</v>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
         <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1051,7 +1051,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15">
         <v>400</v>
@@ -1065,7 +1065,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2">
         <f>C15/(C17*rho*g*C11)*10^6</f>
@@ -1081,7 +1081,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17">
         <v>0.8</v>
@@ -1095,7 +1095,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18">
         <f>12.8/5/100</f>
@@ -1111,7 +1111,7 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -1125,7 +1125,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20">
         <v>0.2</v>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
         <v>81</v>
-      </c>
-      <c r="B23" t="s">
-        <v>82</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1181,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24">
         <v>0.1</v>
@@ -1239,7 +1239,7 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28">
         <v>90</v>
@@ -1253,7 +1253,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="3">
         <f>C13/1000</f>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30">
         <v>0.8</v>
@@ -1282,7 +1282,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1296,7 +1296,7 @@
         <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="2">
         <f>C31/(C33^(-1)*rho*g*C11)*10^6</f>
@@ -1311,7 +1311,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <v>0.8</v>
@@ -1325,7 +1325,7 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34">
         <f>12.8/5/100</f>

</xml_diff>

<commit_message>
clarification in nomenclature of f_reg and d_min in Excel sheet
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6E3016-6ECC-4688-9A7A-405F5D89763B}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62F5C903-7015-4DDF-B983-D5143A9CCF78}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -280,9 +280,6 @@
     <t>[if using pumped storage assessment] pump ramp rate in % of full capacity / min</t>
   </si>
   <si>
-    <t>this percentile controls the amount of allowed VRE overproduction</t>
-  </si>
-  <si>
     <t>fraction of lake volume at which production stops</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>f_reg</t>
   </si>
   <si>
-    <t>[leave empty if unsure - default will be used] which fraction of the water is allocatable for regulated use</t>
-  </si>
-  <si>
     <t>allowed Loss of Energy Expectation as percentage of yearly ELCC</t>
   </si>
   <si>
@@ -310,9 +304,6 @@
     <t>V_lower_initial_frac</t>
   </si>
   <si>
-    <t>minimum required environmental outflow fraction of average inflow (eq. S4, S5)</t>
-  </si>
-  <si>
     <t>represents number of years of filling as threshold for determining f_reg if left unspecified by user (see sheet "Hydropower plant parameters"). Default/recommended is unity, so f_reg represents the fraction of annual mean inflow that would take exactly one year to fill reservoir.</t>
   </si>
   <si>
@@ -359,13 +350,35 @@
   </si>
   <si>
     <t>fraction of solar in the solar/wind portfolio</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">which fraction of the incoming water is allocated for regulated use </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if unsure - default determined by storage size will be used]</t>
+    </r>
+  </si>
+  <si>
+    <t>which fraction of the regulated use (line above) must be dispatched at stable level (eq. S4, S5)</t>
+  </si>
+  <si>
+    <t>this percentile controls the amount of allowed VRE overproduction (represents the % of time in which hydro+VRE may not exceed average ELCC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +387,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -767,13 +788,13 @@
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -806,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -817,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -828,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +862,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,7 +876,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
         <v>20</v>
@@ -866,10 +887,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -880,10 +901,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -894,10 +915,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -908,10 +929,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -922,10 +943,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -936,10 +957,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -950,10 +971,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -964,10 +985,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -981,7 +1002,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1034,10 +1055,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1111,7 +1132,7 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -1125,7 +1146,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20">
         <v>0.2</v>
@@ -1164,10 +1185,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1181,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C24">
         <v>0.1</v>
@@ -1239,7 +1260,7 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C28">
         <v>90</v>
@@ -1265,10 +1286,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <v>0.8</v>

</xml_diff>

<commit_message>
added turbine use statistics capabilities to plotting code + a few cosmetics
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62F5C903-7015-4DDF-B983-D5143A9CCF78}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89DBB7DA-FA88-4781-8C44-5D663929D8D7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t>year_start</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>this percentile controls the amount of allowed VRE overproduction (represents the % of time in which hydro+VRE may not exceed average ELCC)</t>
+  </si>
+  <si>
+    <t>no_turbines</t>
+  </si>
+  <si>
+    <t>number of turbines (units)</t>
   </si>
 </sst>
 </file>
@@ -859,10 +865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,224 +1095,224 @@
         <v>72</v>
       </c>
       <c r="C16" s="2">
-        <f>C15/(C17*rho*g*C11)*10^6</f>
+        <f>C15/(C18*rho*g*C11)*10^6</f>
         <v>637.1049949031601</v>
       </c>
       <c r="D16" s="2">
-        <f>D15/(D17*rho*g*D11)*10^6</f>
+        <f>D15/(D18*rho*g*D11)*10^6</f>
         <v>582.39514769540949</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="C17">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>0.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18">
+        <v>0.8</v>
+      </c>
+      <c r="D18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19">
-        <v>0.1</v>
-      </c>
-      <c r="D19">
-        <v>0.1</v>
-      </c>
-    </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D20">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C21">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D21">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="D22">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="D23">
-        <v>0.74765197999999999</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0.1</v>
+        <v>0.74765197999999999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25">
+        <v>0.1</v>
+      </c>
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26">
-        <v>10</v>
-      </c>
-    </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D27">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="C28">
-        <v>90</v>
+        <v>0.1</v>
       </c>
       <c r="D28">
-        <v>90</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C30" s="3">
         <f>C13/1000</f>
         <v>12570000</v>
       </c>
-      <c r="D29" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30">
-        <v>0.8</v>
-      </c>
       <c r="D30" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="D31" t="e">
         <v>#N/A</v>
@@ -1314,14 +1320,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="2">
-        <f>C31/(C33^(-1)*rho*g*C11)*10^6</f>
-        <v>101.9367991845056</v>
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
       </c>
       <c r="D32" t="e">
         <v>#N/A</v>
@@ -1329,30 +1334,45 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33">
-        <v>0.8</v>
-      </c>
-      <c r="D33">
-        <v>0.8</v>
+        <v>71</v>
+      </c>
+      <c r="C33" s="2">
+        <f>C32/(C34^(-1)*rho*g*C11)*10^6</f>
+        <v>101.9367991845056</v>
+      </c>
+      <c r="D33" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34">
+        <v>0.8</v>
+      </c>
+      <c r="D34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>15</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>76</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
added default calculation of d_min to allow user to leave unspecified
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89DBB7DA-FA88-4781-8C44-5D663929D8D7}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63EBE07E-7A37-482D-B7E4-80EA43C19BD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
   <si>
     <t>year_start</t>
   </si>
@@ -256,30 +256,12 @@
     <t>installed capacity in MW</t>
   </si>
   <si>
-    <t>[if using pumped storage assessment] lower lake volume in m^3</t>
-  </si>
-  <si>
-    <t>[if using pumped storage assessment] pump capacity in MW</t>
-  </si>
-  <si>
-    <t>[if using pumped storage assessment] pump maximum discharge in m^3/s</t>
-  </si>
-  <si>
-    <t>turbine maximum discharge in m^3/s</t>
-  </si>
-  <si>
     <t>turbine efficiency as fraction</t>
   </si>
   <si>
     <t>turbine ramp rate in % of full capacity / min</t>
   </si>
   <si>
-    <t>[if using pumped storage assessment] pump efficiency as fraction</t>
-  </si>
-  <si>
-    <t>[if using pumped storage assessment] pump ramp rate in % of full capacity / min</t>
-  </si>
-  <si>
     <t>fraction of lake volume at which production stops</t>
   </si>
   <si>
@@ -298,9 +280,6 @@
     <t>initial filling fraction of lake volume</t>
   </si>
   <si>
-    <t>[if using pumped storage assessment] initial filling fraction of lower lake volume</t>
-  </si>
-  <si>
     <t>V_lower_initial_frac</t>
   </si>
   <si>
@@ -334,9 +313,6 @@
     <t>HPP_name_data_precipitation</t>
   </si>
   <si>
-    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data</t>
-  </si>
-  <si>
     <t>name of hydropower plant in simulation</t>
   </si>
   <si>
@@ -352,11 +328,42 @@
     <t>fraction of solar in the solar/wind portfolio</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">which fraction of the incoming water is allocated for regulated use </t>
-    </r>
+    <t>this percentile controls the amount of allowed VRE overproduction (represents the % of time in which hydro+VRE may not exceed average ELCC)</t>
+  </si>
+  <si>
+    <t>no_turbines</t>
+  </si>
+  <si>
+    <t>number of turbines (units)</t>
+  </si>
+  <si>
+    <t>maximum discharge (total of all turbines) in m^3/s</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly load normalised to a mean of unity)</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (precipitation flux in kg/m^2/s; hours in rows, years in columns)</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (evaporation flux in kg/m^2/s; hours in rows, years in columns)</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly wind CF as fraction/percentage; hours in rows, years in columns)</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (hourly solar CF as fraction/percentage; hours in rows, years in columns)</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data on reservoir inflow (hourly inflow in m^3/s; hours in rows, years in columns)</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data (first column: volume in m^3; second: surface area in m^2; third: head in m)</t>
+  </si>
+  <si>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="11"/>
         <color theme="1"/>
@@ -366,18 +373,190 @@
       </rPr>
       <t>[leave empty if unsure - default determined by storage size will be used]</t>
     </r>
-  </si>
-  <si>
-    <t>which fraction of the regulated use (line above) must be dispatched at stable level (eq. S4, S5)</t>
-  </si>
-  <si>
-    <t>this percentile controls the amount of allowed VRE overproduction (represents the % of time in which hydro+VRE may not exceed average ELCC)</t>
-  </si>
-  <si>
-    <t>no_turbines</t>
-  </si>
-  <si>
-    <t>number of turbines (units)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which fraction of the incoming water is allocated for regulated use</t>
+    </r>
+  </si>
+  <si>
+    <t>minimum load on one single turbine to ensure high-efficiency range (%)</t>
+  </si>
+  <si>
+    <t>min_load_turbine</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if not using pumped storage assessment]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lower lake volume in m^3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if not using pumped storage assessment]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> initial filling fraction of lower lake volume</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[leave empty if not using pumped storage assessment] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pump capacity in MW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if not using pumped storage assessment]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pump maximum discharge in m^3/s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if not using pumped storage assessment]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pump efficiency as fraction</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[leave empty if not using pumped storage assessment]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pump ramp rate in % of full capacity / min</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [leave empty if unsure - default determined by minimum turbine load will be used]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which fraction of the regulated use (two lines above) must be dispatched at stable level (eq. S4, S5)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -400,6 +579,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -443,6 +623,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
@@ -794,13 +976,13 @@
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -833,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -844,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -855,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -865,16 +1047,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.90625" customWidth="1"/>
-    <col min="2" max="2" width="47.7265625" customWidth="1"/>
+    <col min="2" max="2" width="54.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -882,7 +1064,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
         <v>20</v>
@@ -893,10 +1075,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -907,10 +1089,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -921,10 +1103,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -935,10 +1117,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
+        <v>83</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -949,10 +1131,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" t="s">
-        <v>95</v>
+        <v>84</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -963,10 +1145,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -977,10 +1159,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -991,10 +1173,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1008,7 +1190,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1061,10 +1243,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1092,7 +1274,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2">
         <f>C15/(C18*rho*g*C11)*10^6</f>
@@ -1105,10 +1287,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1122,7 +1304,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C18">
         <v>0.8</v>
@@ -1136,7 +1318,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C19">
         <f>12.8/5/100</f>
@@ -1152,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20">
         <v>0.1</v>
@@ -1166,7 +1348,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C21">
         <v>0.2</v>
@@ -1203,12 +1385,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>101</v>
+        <v>73</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1219,160 +1401,155 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25">
+      <c r="B26" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26">
         <v>0.1</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>10</v>
-      </c>
-    </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D28">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="C29">
-        <v>90</v>
+        <v>0.1</v>
       </c>
       <c r="D29">
-        <v>90</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="3">
+      <c r="B31" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="3">
         <f>C13/1000</f>
         <v>12570000</v>
       </c>
-      <c r="D30" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31">
+    </row>
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32">
         <v>0.8</v>
       </c>
-      <c r="D31" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32">
+      <c r="B33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33">
         <v>100</v>
       </c>
-      <c r="D32" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="2">
-        <f>C32/(C34^(-1)*rho*g*C11)*10^6</f>
+      <c r="B34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="2">
+        <f>C33/(C35^(-1)*rho*g*C11)*10^6</f>
         <v>101.9367991845056</v>
       </c>
-      <c r="D33" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>5</v>
       </c>
-      <c r="B34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34">
+      <c r="B35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35">
         <v>0.8</v>
       </c>
-      <c r="D34">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>15</v>
       </c>
-      <c r="B35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35">
-        <f>12.8/5/100</f>
-        <v>2.5600000000000001E-2</v>
-      </c>
-      <c r="D35">
+      <c r="B36" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
adapting simulation settings file to default d_min calculation
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="228" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63EBE07E-7A37-482D-B7E4-80EA43C19BD0}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE2CE18-E34D-4076-B409-4D40E94FAFCB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -1049,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1419,12 +1419,6 @@
       </c>
       <c r="B26" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C26">
-        <v>0.1</v>
-      </c>
-      <c r="D26">
-        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added calculation of guaranteed power based on exceedance probability
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE2CE18-E34D-4076-B409-4D40E94FAFCB}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87BA33E8-92C7-4969-9AC8-788D09AE5859}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="116">
   <si>
     <t>year_start</t>
   </si>
@@ -557,6 +557,12 @@
       </rPr>
       <t xml:space="preserve"> which fraction of the regulated use (two lines above) must be dispatched at stable level (eq. S4, S5)</t>
     </r>
+  </si>
+  <si>
+    <t>this percentile is used to calculate the exceedance probability of delivered power (guaranteed capacity, MW). For P90, use 90; for P95, use 95, etc.</t>
+  </si>
+  <si>
+    <t>p_exceedance</t>
   </si>
 </sst>
 </file>
@@ -615,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -623,7 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -641,6 +646,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -943,7 +952,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1091,7 +1100,7 @@
       <c r="A3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>102</v>
       </c>
       <c r="C3" t="s">
@@ -1105,7 +1114,7 @@
       <c r="A4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>101</v>
       </c>
       <c r="C4" t="s">
@@ -1119,7 +1128,7 @@
       <c r="A5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>100</v>
       </c>
       <c r="C5" t="s">
@@ -1133,7 +1142,7 @@
       <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>99</v>
       </c>
       <c r="C6" t="s">
@@ -1147,7 +1156,7 @@
       <c r="A7" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>98</v>
       </c>
       <c r="C7" t="s">
@@ -1161,7 +1170,7 @@
       <c r="A8" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>97</v>
       </c>
       <c r="C8" t="s">
@@ -1175,7 +1184,7 @@
       <c r="A9" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>103</v>
       </c>
       <c r="C9" t="s">
@@ -1392,12 +1401,6 @@
       <c r="B24" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>0.74765197999999999</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -1406,10 +1409,10 @@
       <c r="B25" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>0.35</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>0.35</v>
       </c>
     </row>
@@ -1479,71 +1482,85 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31">
+        <v>90</v>
+      </c>
+      <c r="D31">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C32" s="3">
         <f>C13/1000</f>
         <v>12570000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32">
-        <v>0.8</v>
-      </c>
-    </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33">
-        <v>100</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="2">
-        <f>C33/(C35^(-1)*rho*g*C11)*10^6</f>
-        <v>101.9367991845056</v>
+        <v>109</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35">
-        <v>0.8</v>
+        <v>110</v>
+      </c>
+      <c r="C35" s="2">
+        <f>C34/(C36^(-1)*rho*g*C11)*10^6</f>
+        <v>101.9367991845056</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
@@ -1559,7 +1576,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
explicitly included possibility to specify irrigation requirements and environmental flow separately from minimum turbine load constraints
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87BA33E8-92C7-4969-9AC8-788D09AE5859}"/>
+  <xr:revisionPtr revIDLastSave="287" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C02951-12B0-4180-8D92-66F872B9175B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
   <si>
     <t>year_start</t>
   </si>
@@ -563,6 +563,12 @@
   </si>
   <si>
     <t>p_exceedance</t>
+  </si>
+  <si>
+    <t>HPP_name_data_outflow_prescribed</t>
+  </si>
+  <si>
+    <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data on prescribed (environmental/irrigation) outflow (hourly in m^3/s; hours in rows, years in columns)</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1112,10 +1118,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1126,10 +1132,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1140,10 +1146,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1154,10 +1160,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1168,10 +1174,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -1182,10 +1188,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1196,298 +1202,298 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>36.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="1">
-        <v>440000000</v>
-      </c>
-      <c r="D12" s="1">
-        <v>900000000</v>
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>36.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1">
-        <v>12570000000</v>
+        <v>440000000</v>
       </c>
       <c r="D13" s="1">
-        <v>8300000000</v>
+        <v>900000000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14">
-        <v>0.8</v>
-      </c>
-      <c r="D14">
-        <v>0.8</v>
+        <v>67</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12570000000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8300000000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C15">
-        <v>400</v>
+        <v>0.8</v>
       </c>
       <c r="D15">
-        <v>165</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="2">
-        <f>C15/(C18*rho*g*C11)*10^6</f>
-        <v>637.1049949031601</v>
-      </c>
-      <c r="D16" s="2">
-        <f>D15/(D18*rho*g*D11)*10^6</f>
-        <v>582.39514769540949</v>
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+      <c r="D16">
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
+        <v>96</v>
+      </c>
+      <c r="C17" s="2">
+        <f>C16/(C19*rho*g*C12)*10^6</f>
+        <v>637.1049949031601</v>
+      </c>
+      <c r="D17" s="2">
+        <f>D16/(D19*rho*g*D12)*10^6</f>
+        <v>582.39514769540949</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C18">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>0.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19">
+        <v>0.8</v>
+      </c>
+      <c r="D19">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20">
-        <v>0.1</v>
-      </c>
-      <c r="D20">
-        <v>0.1</v>
-      </c>
-    </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D21">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C22">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D22">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>0.8</v>
+      </c>
+      <c r="D23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>0.95</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>0.95</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>106</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>0.35</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D26" s="5">
         <v>0.35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>34</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28">
-        <v>10</v>
-      </c>
-      <c r="D28">
-        <v>10</v>
-      </c>
-    </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D29">
-        <v>0.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="C30">
-        <v>90</v>
+        <v>0.1</v>
       </c>
       <c r="D30">
-        <v>90</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C31">
         <v>90</v>
@@ -1496,71 +1502,85 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="3">
-        <f>C13/1000</f>
-        <v>12570000</v>
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32">
+        <v>90</v>
+      </c>
+      <c r="D32">
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33">
-        <v>0.8</v>
+        <v>107</v>
+      </c>
+      <c r="C33" s="3">
+        <f>C14/1000</f>
+        <v>12570000</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34">
-        <v>100</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="2">
-        <f>C34/(C36^(-1)*rho*g*C11)*10^6</f>
-        <v>101.9367991845056</v>
+        <v>109</v>
+      </c>
+      <c r="C35">
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36">
-        <v>0.8</v>
+        <v>110</v>
+      </c>
+      <c r="C36" s="2">
+        <f>C35/(C37^(-1)*rho*g*C12)*10^6</f>
+        <v>101.9367991845056</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <f>12.8/5/100</f>
         <v>2.5600000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
corrected typo in parameters_simulation file
</commit_message>
<xml_diff>
--- a/data/parameters_simulation.xlsx
+++ b/data/parameters_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/Backup Private/Archive/2018-2021 VUB Work Files/20001 REVUB Python/West Africa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/sebastian_sterl_vub_be/Documents/Documenten/VUB Work Files/REVUB code repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C02951-12B0-4180-8D92-66F872B9175B}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{18519E58-EEB6-42A0-A5AE-E51108518862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9C4A651-C5A5-484B-B7C5-36988BCB04BC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B27AEA38-A928-4B6A-AF9B-7A28216807AA}"/>
   </bookViews>
@@ -385,9 +385,6 @@
     </r>
   </si>
   <si>
-    <t>minimum load on one single turbine to ensure high-efficiency range (%)</t>
-  </si>
-  <si>
     <t>min_load_turbine</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>name of corresponding worksheet in the "data" Excel sheets from which to pull data on prescribed (environmental/irrigation) outflow (hourly in m^3/s; hours in rows, years in columns)</t>
+  </si>
+  <si>
+    <t>minimum load on one single turbine to ensure high-efficiency range (fraction)</t>
   </si>
 </sst>
 </file>
@@ -654,14 +654,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -699,7 +695,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -805,7 +801,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -947,7 +943,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1064,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D23870-37A0-4EFA-BF75-9E0BBC5C39B4}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1118,10 +1114,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
         <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1424,10 +1420,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C26" s="5">
         <v>0.35</v>
@@ -1441,7 +1437,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1504,10 +1500,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C32">
         <v>90</v>
@@ -1521,7 +1517,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="3">
         <f>C14/1000</f>
@@ -1533,7 +1529,7 @@
         <v>77</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34">
         <v>0.8</v>
@@ -1544,7 +1540,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1555,7 +1551,7 @@
         <v>64</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="2">
         <f>C35/(C37^(-1)*rho*g*C12)*10^6</f>
@@ -1567,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>0.8</v>
@@ -1578,7 +1574,7 @@
         <v>15</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <f>12.8/5/100</f>

</xml_diff>